<commit_message>
Changed some super stats to balance out the new powersets
</commit_message>
<xml_diff>
--- a/SupersRules/SuperStats.xlsx
+++ b/SupersRules/SuperStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>STR</t>
   </si>
@@ -193,6 +193,18 @@
   </si>
   <si>
     <t>Psychic Powers</t>
+  </si>
+  <si>
+    <t>Jetpack Flight</t>
+  </si>
+  <si>
+    <t>Occular Powers</t>
+  </si>
+  <si>
+    <t>Plant Control</t>
+  </si>
+  <si>
+    <t>Staff Melee</t>
   </si>
 </sst>
 </file>
@@ -542,11 +554,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q9" sqref="Q9"/>
+      <selection pane="bottomLeft" activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,38 +872,32 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="1">
+        <v>59</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="J24">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -905,142 +911,148 @@
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-      <c r="K27" s="1">
-        <v>1</v>
-      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
-      </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
-      <c r="I28">
-        <v>1</v>
-      </c>
-      <c r="J28" s="1">
+        <v>32</v>
+      </c>
+      <c r="K28" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1">
+        <v>33</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>35</v>
-      </c>
-      <c r="I30">
+        <v>34</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
-      </c>
-      <c r="G31" s="1">
-        <v>1</v>
-      </c>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1">
+        <v>60</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="K31">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-      <c r="K32">
+        <v>61</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="J32">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
-      </c>
-      <c r="E35">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="K35">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>39</v>
-      </c>
-      <c r="K36">
-        <v>1</v>
-      </c>
+      <c r="A36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1055,188 +1067,232 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
-      </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-      <c r="K38">
+        <v>38</v>
+      </c>
+      <c r="E38">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39">
+        <v>39</v>
+      </c>
+      <c r="K39">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
-      <c r="E40">
+      <c r="D40">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="F41">
-        <v>1</v>
-      </c>
+      <c r="A41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
-      </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="H42">
+        <v>42</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="K42">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>47</v>
-      </c>
-      <c r="H43">
+        <v>43</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
-      </c>
-      <c r="G44">
+        <v>44</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="E44">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>56</v>
-      </c>
-      <c r="G45" s="1">
+        <v>45</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="F45">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>49</v>
-      </c>
-      <c r="H46" s="1">
-        <v>1</v>
-      </c>
-      <c r="J46" s="1">
+        <v>46</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="H46">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>57</v>
-      </c>
-      <c r="D47" s="1">
+        <v>47</v>
+      </c>
+      <c r="H47">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="G49" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="H50" s="1">
+        <v>1</v>
+      </c>
+      <c r="J50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="1">
-        <v>1</v>
-      </c>
-      <c r="C50" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B51">
-        <f>SUM(B2:B50)</f>
+      <c r="B54" s="1">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <f>SUM(B2:B54)</f>
         <v>6</v>
       </c>
-      <c r="C51">
-        <f t="shared" ref="C51:K51" si="0">SUM(C2:C50)</f>
-        <v>6</v>
-      </c>
-      <c r="D51">
+      <c r="C55">
+        <f t="shared" ref="C55:K55" si="0">SUM(C2:C54)</f>
+        <v>8</v>
+      </c>
+      <c r="D55">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E51">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G51">
+        <v>8</v>
+      </c>
+      <c r="E55">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H51">
+      <c r="F55">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I51">
+      <c r="G55">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J51">
+      <c r="H55">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="K51">
+        <v>7</v>
+      </c>
+      <c r="I55">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>